<commit_message>
Did my part of the EDA
I added a .csv format instead of xlsx And then did my part for the EDA and knitted the code
</commit_message>
<xml_diff>
--- a/Code/AI in Retail Dataset.xlsx
+++ b/Code/AI in Retail Dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1 -Rathi Backup 20 Oct 2022\Publication\2023\Esra -Paper - 4. Applied AI -Q3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8506a749f9b9ad6c/Documents/Graduate Classes/DSE6311 Capstone/DSE6311-Graduate-DS-Capstone/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAEB76A-3AF2-4778-B7A7-BF4D274F9042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{6AAEB76A-3AF2-4778-B7A7-BF4D274F9042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10253EE9-EDED-41D0-A045-A1553C20D458}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default_1" sheetId="1" r:id="rId1"/>
@@ -253,9 +253,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -293,7 +293,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -399,7 +399,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -541,7 +541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,15 +551,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W657"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added a file that runs LDA
Unsure if this is the right unsupervised method I dont think we need this based on the results Plus based on some reading I did we only have two classes so we cant lower it anymore or else our machine learning models won't work
</commit_message>
<xml_diff>
--- a/Code/AI in Retail Dataset.xlsx
+++ b/Code/AI in Retail Dataset.xlsx
@@ -250,6 +250,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -551,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>